<commit_message>
Add Pagination to GetAllExpense API
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -44,18 +44,6 @@
   </si>
   <si>
     <t>Food</t>
-  </si>
-  <si>
-    <t>e31947c2-b911-437c-960b-352ae8d151e4</t>
-  </si>
-  <si>
-    <t>99e0f392-3fa6-40b6-b69d-5386e052ff2b</t>
-  </si>
-  <si>
-    <t>53685ce8-05fc-405e-9cd2-b96b52ff0e5c</t>
-  </si>
-  <si>
-    <t>this is expense app</t>
   </si>
 </sst>
 </file>
@@ -433,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -480,75 +468,6 @@
       </c>
       <c r="G3" s="1">
         <v>45194.48602372685</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>122</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>45194.48606398148</v>
-      </c>
-      <c r="G4" s="1">
-        <v>45194.48606398148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>1344</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
-        <v>45194.48611063657</v>
-      </c>
-      <c r="G5" s="1">
-        <v>45194.48611063657</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45194.496575625</v>
-      </c>
-      <c r="G6" s="1">
-        <v>45194.496575625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add key and certificates
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -34,22 +34,28 @@
     <t>updatedAt</t>
   </si>
   <si>
-    <t>5b2e5e7b-2430-41ed-81b3-53f27211f287</t>
-  </si>
-  <si>
-    <t>6ed575f9-210b-4302-8f2c-324fc0ee3227</t>
-  </si>
-  <si>
-    <t>this is desciii</t>
+    <t>71f07443-f6a6-4fef-a0a3-93b494e4e3af</t>
+  </si>
+  <si>
+    <t>b68d09e7-df5d-4d13-bee3-ac455e4a33e9</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Food</t>
   </si>
   <si>
-    <t>17600fdf-8b1e-48f4-96e5-18d11d10d4ad</t>
-  </si>
-  <si>
-    <t>this is notyy</t>
+    <t>6574d207-b6e8-4ad4-b1e8-f46ca7f4f0f3</t>
+  </si>
+  <si>
+    <t>20da1323-1d1c-4ec5-9394-2ca5f663702b</t>
+  </si>
+  <si>
+    <t>82e368a2-975e-4b5f-a7cd-3e5982d35bde</t>
+  </si>
+  <si>
+    <t>a013816c-0f7b-44e7-9c76-97cef7f30f1e</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -461,7 +467,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -470,10 +476,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>45196.321418067135</v>
+        <v>45197.28138627315</v>
       </c>
       <c r="G3" s="1">
-        <v>45196.321418067135</v>
+        <v>45197.28138627315</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -484,19 +490,88 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1">
-        <v>45196.32149973379</v>
+        <v>45197.28142216435</v>
       </c>
       <c r="G4" s="1">
-        <v>45196.32149973379</v>
+        <v>45197.28142216435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45197.28147271991</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45197.28147271991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45197.28188016204</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45197.28188016204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45197.28191664352</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45197.28191664352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>